<commit_message>
Data relabelled & result changed
</commit_message>
<xml_diff>
--- a/dataset/combined_pair.xlsx
+++ b/dataset/combined_pair.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajed/PycharmProjects/Study-on-ChatGPT/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9701CEB8-F997-9A41-8C22-AA300B424C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240703DD-5D2E-5640-B7AB-E17C11EAA9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="277">
   <si>
     <t>id</t>
   </si>
@@ -364,9 +364,6 @@
 </t>
   </si>
   <si>
-    <t>Could not find the case where every element occurs once</t>
-  </si>
-  <si>
     <t>This method does not have any potential test cases that would result in an error, but not a failure. The only exception thrown by the method is a `NullPointerException` which is thrown when the input array `x` is null. This exception is thrown before the program counter reaches any other lines of code in the method, so it would be considered a failure.
 Additionally, the implementation of the function is simple and doesn't have any logical error that could prevent it from returning the expected value. It will always return the last index of zero in the array or -1 if the zero is not present. If a test case is passed to this function it will successfully complete its execution by returning the value.
 It is possible that if the array is not of int type then the function would throw an exception but in the given implementation it is clearly mentioned that the input to the function is int array which eliminates this case as well.</t>
@@ -461,9 +458,6 @@
 ```
 Expected Output: `Last zero index: 6`
 If the output match the expectation, you can say that the solution is working fine and also can capture the output in some image and that can be your evidence of the solution working.</t>
-  </si>
-  <si>
-    <t>Although correct, It did not executed the commented test</t>
   </si>
   <si>
     <t>Here is the corrected version of the code that finds the last index of zero in the array:
@@ -525,9 +519,6 @@
 // test: x = [-3, -2, 0, 1, 4]; Expected = 3</t>
   </si>
   <si>
-    <t>Finds the correct issue but fails to give a fix for the code</t>
-  </si>
-  <si>
     <t xml:space="preserve">The given code correctly counts the number of elements in the input array that are either odd or positive. However, it does not properly handle the case where the input array is null, as it will throw a NullPointerException. To fix this, a null check should be added before the for loop to ensure that the input array is not null. Here is one possible modification:
 ```
 public static int oddOrPos (int[] x)
@@ -647,9 +638,6 @@
 It's worth noting that the function has a null check and throws NullPointerException if the input array is null, meaning that passing a null array will result in the fault in this case, which is desirable and expected.</t>
   </si>
   <si>
-    <t>Talks about the empty cases but misses the null case</t>
-  </si>
-  <si>
     <t>A test case that does not execute the fault would be an input array of all even and non-positive integers, such as [0, -2, -4, -6]. The method would return 0 as the count of elements in the array that are either odd or positive is 0.</t>
   </si>
   <si>
@@ -698,9 +686,6 @@
   </si>
   <si>
     <t>A test case that results in an error would be passing a null value for the parameter x, as the method throws a NullPointerException in this case. This is not a failure as the method is correctly handling the error condition by throwing an exception.</t>
-  </si>
-  <si>
-    <t>Did not talk about the commented test case</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -764,9 +749,6 @@
 ```if (x[i] % 2 != 0 || x[i] &gt; 0)``` 
 The current if statement check for x[i] &gt; 0 but in case the element is negative and even it will be considered as not odd or positive. But if we use above if statement it will take care of even positive numbers too.
 Please verify the output for the given test cases and consider it as a evidence for the new program working.</t>
-  </si>
-  <si>
-    <t>Finds a solution that the writer did not talk about</t>
   </si>
   <si>
     <t>I'm sorry, I am an AI language model and do not have the capability to execute code or take screenshots. However, based on the provided code, it looks like the function "oddOrPos" is counting the number of elements in the input array "x" that are either odd or positive. The given test case, where x = [-3, -2, 0, 1, 4], should return 3 as there are 3 elements (1, -2 and 4) that are either odd or positive in the array x. If this test case returns the expected output, then the function should be working correctly.</t>
@@ -959,11 +941,6 @@
 This test case demonstrates the inconsistency between equals() and compareTo() in the BigDecimal class, but it does not result in an error state as the program runs successfully.</t>
   </si>
   <si>
-    <t>In the given example, the problem is that the BigDecimal class's equals() and compareTo() methods are inconsistent. The code creates two BigDecimal objects, x and y, with the values "1.0" and "1.00" respectively. Even though x and y are not equal according to the equals() method (!x.equals(y)), the compareTo() method returns 0, indicating that they are equal.
-When these objects are added to a TreeSet, the set uses the compareTo() method to determine equality, so only one element is added to the set. However, when added to a HashSet, the set uses the equals() method, so both x and y are added to the set.
-A test case that executes this fault but does not result in an error state would be to create two BigDecimal objects with slightly different values, and add them to both a TreeSet and a HashSet. The output of the test would show that the TreeSet only has one element, while the HashSet has two elements, which would demonstrate the inconsistency between the equals() and compareTo() methods in the BigDecimal class.</t>
-  </si>
-  <si>
     <t>If possible, give a test case that results in an error, but not a failure. If not, briefly explain why not. Hint: Don’t forget about the program counter.</t>
   </si>
   <si>
@@ -986,9 +963,6 @@
 </t>
   </si>
   <si>
-    <t>Treats error equavalent to exception</t>
-  </si>
-  <si>
     <t>The code you've provided is an example of a class that demonstrates a problem with the `BigDecimal` class, specifically the inconsistency between its `equals()` and `compareTo()` methods. In this example, `x` and `y` are two `BigDecimal` objects that have the same value but are not considered equal by the `equals()` method. 
 The code creates two sets, `BigDecimalTree` and `BigDecimalHash`, both of which are initialized with the `x` and `y` values. However, because `TreeSet` uses the `compareTo()` method for ordering elements and determining uniqueness, and `HashSet` uses the `equals()` method, the two sets end up with different numbers of elements. 
 In order to demonstrate a case which result in an error, but not a failure one can try use BigDecimal to write a program that performs some computation and compares the results of the computation to an expected value. 
@@ -1015,9 +989,6 @@
 </t>
   </si>
   <si>
-    <t>Wrong assumption by chatGPT</t>
-  </si>
-  <si>
     <t>The first error state in the given code is that the `BigDecimalTree` Set only contains one element (1.0) instead of two (1.0 and 1.00) as expected. This is because the `TreeSet` class uses the `compareTo()` method to determine equality of elements, whereas the `BigDecimal` class has an inconsistent implementation of `compareTo()` and `equals()`, such that `x.compareTo(y) == 0` but `!x.equals(y)`. Since `x` and `y` are not considered equal according to `equals()`, they are both added to the `BigDecimalTree` Set, resulting in only one element in the set.</t>
   </si>
   <si>
@@ -1025,9 +996,6 @@
   </si>
   <si>
     <t>The first error state in the given code occurs when the elements x and y, which are instances of the BigDecimal class with the values "1.0" and "1.00" respectively, are added to the BigDecimalTree Set. Since the TreeSet uses the compareTo() method for comparison, the element y is considered equal to the element x and is not added to the set, resulting in the BigDecimalTree Set having only 1 element. This is an error state as the expected behavior is that the BigDecimalTree Set should have 2 elements, x and y, as they have different values.</t>
-  </si>
-  <si>
-    <t>Writer differs in the sense that it is a part of JAVA API and cannot be modified without consequences in the client code all over the world. But chatGPT provides a fix that would be the soultion if it was written properly.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1191,9 +1159,6 @@
 </t>
   </si>
   <si>
-    <t>There will be no valid code solution</t>
-  </si>
-  <si>
     <t>The class `ColorPoint` is a subclass of `Point`, and it extends the state of the `Point` class by adding a color field. However, the implementation of the `equals` method in the `ColorPoint` class fails to take this into account.
 In the `equals` method at Location B, it first checks if the object passed in is an instance of `ColorPoint` using the `instanceof` operator. If it is not, it immediately returns `false`. This means that a `Point` object and a `ColorPoint` object with the same x and y coordinates will be considered not equal, even though they should be.
 To fix this, the check at Location B should be modified to check if the passed in object is an instance of `Point` instead of `ColorPoint`. This way, a `Point` object and a `ColorPoint` object with the same x and y coordinates will be considered equal. Additionally, `ColorPoint` should override `hashCode` method if it also overrode `equals` to be compliant with general contract for `hashCode()` and `equals()`
@@ -1225,9 +1190,6 @@
 By doing this, `equals` would now correctly handle the case where it is passed an object of a superclass, and the above test cases would produce the expected results.</t>
   </si>
   <si>
-    <t>Talks about hashcode which the author missed</t>
-  </si>
-  <si>
     <t>The given code contains a fault in the implementation of the equals method in the ColorPoint class. The problem is that the subclass, ColorPoint, extends the state of the superclass, Point, by adding a color field, but it does not override the equals method of the superclass to take this additional state into account.
 To fix this fault, the equals method in the ColorPoint class should be modified to check if the objects being compared are instances of the same class, and then check the color field in addition to the x and y fields inherited from the Point class.
 A possible modification to the code would be:
@@ -1278,9 +1240,6 @@
 p1.equals(p2); // Result = true
 ```
 As you can see, this test case does not execute the fault because it does not involve any instances of the `ColorPoint` class.</t>
-  </si>
-  <si>
-    <t>Talks about the problem in both equals()</t>
   </si>
   <si>
     <t>The class ColorPoint extends Point, and adds the additional state of 'color'. The class overrides the equals method, but the implementation is faulty as it only compares the color state of the ColorPoint class, it does not consider the Point class' state of x and y. In the test cases, p.equals(cp1) returns true, but cp1.equals(p) returns false, and cp1.equals(cp2) also returns false, while they are expected to return true.
@@ -1382,9 +1341,6 @@
   <si>
     <t>The first error state in the given code is in the implementation of the `equals` method in the `ColorPoint` class. The implementation overrides the `equals` method inherited from the `Point` class, but it only returns `true` if the passed-in object is an instance of `ColorPoint` and if the color of the two objects match. This means that if an instance of `Point` is passed to the `equals` method of an instance of `ColorPoint`, the method will always return `false`, even if the x and y coordinates of the two points are the same. This violates the symmetric and transitive requirements of the `equals` method, as described in the `Object` class.
 Another error state in the given code is the class hierarchy, `ColorPoint` extends `Point` and `Point` is instantiable and the subclass state is extended by adding `color` attribute. This design decision can lead to many issues like tests 1 and 2 returning different results, whereas they should return the same results.</t>
-  </si>
-  <si>
-    <t>Also talks about design perspective</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1483,9 +1439,6 @@
 I hope this helps!</t>
   </si>
   <si>
-    <t>Talks about composition indirectly</t>
-  </si>
-  <si>
     <t>The class Point defines a simple class that represents a point in 2D space. It has two private instance variables, x and y, that represent the x and y coordinates of the point. The class has a constructor that initializes these variables and an equals method that compares the x and y coordinates of this point with another point object.
 The class ColorPoint is a subclass of Point. It extends the state of the Point class by adding a private instance variable, color, that represents the color of the point. The class has a constructor that calls the constructor of the superclass and initializes the color variable. It also overrides the equals method of the superclass to include a comparison of the color instance variable in addition to the x and y coordinates.
 The fault in this class hierarchy is that the equals method in the ColorPoint class does not properly handle the case when it is passed a Point object instead of a ColorPoint object. The current implementation returns false in that case, which is incorrect. The expected behavior is that the equals method should return true when a Point object and a ColorPoint object have the same x and y coordinates, regardless of the color of the ColorPoint object.
@@ -1855,9 +1808,6 @@
     <t>Rewrite your JUnit test as an appropriate JUnit theory. Evaluate it with suitable DataPoints.</t>
   </si>
   <si>
-    <t>Does not consider null points, non-point objects</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Here is an example of the JUnit test from (c) rewritten as a JUnit theory using appropriate DataPoints:
 ```java
@@ -2072,19 +2022,6 @@
     <t>Treats error as exception/crash</t>
   </si>
   <si>
-    <t xml:space="preserve">The first error state for the test case where a null value is passed to the function as an argument, for example:
-Copy code
-lastZero(null);
-The error state is a NullPointerException being thrown. This error state occurs when the code attempts to access elements of the input array, but the array is null, so the program throws an exception.
-The complete state of the error would be:
-The program counter is pointing at the line where the exception is thrown
-The exception message is "null"
-The stack trace will show the method lastZero(int[] x) as the location where the exception occurred
-The program continues to execute other lines of code after catching the exception, if it is handled properly.
-It is worth noting that this error state is handled explicitly by the code, it will throw the exception if the input is null, so it is not a failure but it is an error.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">As I mentioned previously, there are multiple ways to fix the original code and make it work as expected. But, I will show one possible way to fix the original code and make it return the last index of zero.
 Copy code
 public static int lastZero (int[] x) {
@@ -2141,90 +2078,8 @@
 In this case, the program will stop execution when the exception is thrown, hence it is not possible to have a test case that results in an error but not a failure.</t>
   </si>
   <si>
-    <t>The given test case is:
-Copy code
-int[] x = {-3, -2, 0, 1, 4};
-int result = oddOrPos(x);
-assert result == 3;
-In this test case, the first error state would not occur because the input array x is non-null. The method implementation includes a null check to check if the input array is null or not, if it is null it will throw a NullPointerException. Since the input array is non-null, the method will execute as expected and the first error state will not occur.
-It is worth noting that the test case also includes an assertion that compares the returned result from the method with the expected value of 3, if the returned value is not 3 it will result in an assertion error and the program will stop execution.</t>
-  </si>
-  <si>
     <t>Treats error as exception/crash
 Detects test from the commented code</t>
-  </si>
-  <si>
-    <t>Here is an implementation of the repaired code that includes a null check for the input array:
-Copy code
-public static int oddOrPos (int[] x) {
-      if (x == null) {
-         throw new NullPointerException("Input array cannot be null");
-      }
-      int count = 0;
-      for (int i = 0; i &lt; x.length; i++) {
-         if (x[i]%2 == 1 || x[i] &gt; 0) {
-            count++;
-         }
-      }
-      return count;
-   }
-And here is the test case that verifies that the given test now produces the expected output:
-Copy code
-int[] x = {-3, -2, 0, 1, 4};
-int result = oddOrPos(x);
-assert result == 3;
-As you can see, the method now includes a null check for the input array, which will ensure that the method will throw a NullPointerException if a null array is passed as an input. The test case that is provided will pass as the input array is non-null and the expected output is 3 which is being asserted against the returned result.
-In addition, if you are running this code on a Java development environment such as eclipse, it will give you a message that the test passed and you can see it on the console.</t>
-  </si>
-  <si>
-    <t>The given code uses the BigDecimal class, which has an inconsistency between its equals() and compareTo() methods. Specifically, x.equals(y) returns false, but x.compareTo(y) returns 0, indicating that they are equal. This inconsistency causes problems when using BigDecimal objects with certain types of collections, such as TreeSet and HashSet.
-In the given code, a TreeSet is created and both x and y are added to it. Since TreeSet uses the compareTo() method for ordering and comparison, the two BigDecimal objects are considered equal and only one element is added to the set. On the other hand, a HashSet is created and both x and y are added to it. Since HashSet uses the equals() method for comparison, the two BigDecimal objects are considered different and both are added to the set.
-To fix this fault, one approach would be to override the equals() method in the BigDecimal class to use the compareTo() method instead. Alternatively, a custom comparator that uses the compareTo() method could be provided when creating the TreeSet and HashSet collections.
-For example:
-Copy code
-public class BigDecimalTest {
-    BigDecimal x = new BigDecimal ("1.0");
-    BigDecimal y = new BigDecimal ("1.00");
-    //override equals method
-    @Override
-    public boolean equals(Object obj) {
-        if(obj instanceof BigDecimal) {
-            return this.compareTo((BigDecimal) obj) == 0;
-        }
-        return false;
-    }
-    // Fact: x.equals (y) should now return true, and x.compareTo (y) == 0
-    Set &lt;BigDecimal&gt; BigDecimalTree = new TreeSet &lt;BigDecimal&gt; ();
-    BigDecimalTree.add (x);
-    BigDecimalTree.add (y);
-    // TreeSet uses compareTo(), so BigDecimalTree will now have 1 element
-    Set &lt;BigDecimal&gt; BigDecimalHash = new HashSet &lt;BigDecimal&gt; ();
-    BigDecimalHash.add (x);
-    BigDecimalHash.add (y);
-    // HashSet uses equals(), so BigDecimalHash will now have 1 element
-    }
-    // Test: System.out.println ("BigDecimalTree = " + BigDecimalTree);
-    // System.out.println ("BigDecimalHash = " + BigDecimalHash);
-    // Expected: BigDecimalTree = 1; BigDecimalHash = 1
-    // See Java Doc for add() in Set Interface
-This modification will ensure that the equals() method will return true when comparing x and y and fix the inconsistency between equals() and compareTo() methods in the BigDecimal class.</t>
-  </si>
-  <si>
-    <t>It is not possible to give a test case that does not execute the fault because the fault is inherent in the way that the BigDecimal class is implemented. The equals() and compareTo() methods in the BigDecimal class return different results for certain values, which causes problems when using BigDecimal objects with certain types of collections, such as TreeSet and HashSet.
-However, once the equals method is overriden as described in (a) with the compareTo method, the test case will be successful.
-For example:
-Copy code
-BigDecimal x = new BigDecimal ("1.0");
-BigDecimal y = new BigDecimal ("1.00");
-Set &lt;BigDecimal&gt; BigDecimalTree = new TreeSet &lt;BigDecimal&gt; ();
-BigDecimalTree.add (x);
-BigDecimalTree.add (y);
-assertEquals(1,BigDecimalTree.size());
-Set &lt;BigDecimal&gt; BigDecimalHash = new HashSet &lt;BigDecimal&gt; ();
-BigDecimalHash.add (x);
-BigDecimalHash.add (y);
-assertEquals(1,BigDecimalHash.size());
-In this test case, the size of BigDecimalTree and BigDecimalHash should be 1, this means that only one element is added to each of them, which is expected.</t>
   </si>
   <si>
     <t>It is possible to give a test case that executes the fault, but does not result in an error state.
@@ -2256,53 +2111,6 @@
 The program runs without crashing, but the output is not what is expected. This is a failure but not an error.</t>
   </si>
   <si>
-    <t>Did not talk about the exact line
-Treats error as exception/crash</t>
-  </si>
-  <si>
-    <t>As I mentioned before, one approach to repair the fault in the code is to override the equals() method in the BigDecimal class to use the compareTo() method instead.
-Here is the modified code:
-Copy code
-public class BigDecimalTest {
-    BigDecimal x = new BigDecimal ("1.0");
-    BigDecimal y = new BigDecimal ("1.00");
-    //override equals method
-    @Override
-    public boolean equals(Object obj) {
-        if(obj instanceof BigDecimal) {
-            return this.compareTo((BigDecimal) obj) == 0;
-        }
-        return false;
-    }
-    // Fact: x.equals (y) should now return true, and x.compareTo (y) == 0
-    Set &lt;BigDecimal&gt; BigDecimalTree = new TreeSet &lt;BigDecimal&gt; ();
-    BigDecimalTree.add (x);
-    BigDecimalTree.add (y);
-    // TreeSet uses compareTo(), so BigDecimalTree will now have 1 element
-    Set &lt;BigDecimal&gt; BigDecimalHash = new HashSet &lt;BigDecimal&gt; ();
-    BigDecimalHash.add (x);
-    BigDecimalHash.add (y);
-    // HashSet uses equals(), so BigDecimalHash will now have 1 element
-    }
-    // Test: System.out.println ("BigDecimalTree = " + BigDecimalTree);
-    // System.out.println ("BigDecimalHash = " + BigDecimalHash);
-    // Expected: BigDecimalTree = 1; BigDecimalHash = 1
-With this modification, the test case that was provided will now produce the expected output.
-Copy code
-BigDecimal x = new BigDecimal ("1.0");
-BigDecimal y = new BigDecimal ("1.00");
-Set &lt;BigDecimal&gt; BigDecimalTree = new TreeSet &lt;BigDecimal&gt; ();
-BigDecimalTree.add (x);
-BigDecimalTree.add (y);
-assertEquals(1,BigDecimalTree.size());
-Set &lt;BigDecimal&gt; BigDecimalHash = new HashSet &lt;BigDecimal&gt; ();
-BigDecimalHash.add (x);
-BigDecimalHash.add (y);
-assertEquals(1,BigDecimalHash.size());
-In this test case, the size of BigDecimalTree and BigDecimalHash should be 1, this means that only one element is added to each of them, which is expected.
-I apologize but as a language model AI I am not able to provide you with a screenshot or any other evidence, but you can run the code and see that it works as expected.</t>
-  </si>
-  <si>
     <t>Detects test from the commented code
 Writer differs in the sense that it is a part of JAVA API and cannot be modified without consequences in the client code all over the world. But chatGPT provides a fix that would be the soultion if it was written properly.</t>
   </si>
@@ -2328,19 +2136,6 @@
 ColorPoint cp1 = new ColorPoint (1,2,RED);
 p.equals (cp1);
 the fault will still be executed since the equals method in ColorPoint class does not check for equality of color field and it will return false.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It is possible to give a test case that executes the fault but does not result in an error state.
-For example, the following test case:
-Copy code
-Point p = new Point (1,2);
-ColorPoint cp1 = new ColorPoint (1,2,RED);
-ColorPoint cp2 = new ColorPoint (1,2,BLUE);
-p.equals (cp1); // Test 1: Result = true;
-This test case will execute the fault because the equals method in the ColorPoint class does not properly check for equality of all relevant fields, including the color field, when comparing ColorPoint objects. However, it does not result in an error state because the result of the comparison is true.
-This is because the equals method of Point class is being used to compare the Point and ColorPoint object, it checks for equality of x and y fields and hence the comparison returns true.
-Even though this test case does not result in an error state, it is still problematic because it can lead to unexpected behavior and bugs in the program, as it is returning true when it should be false.
-</t>
   </si>
   <si>
     <t>Detects test from the commented code
@@ -2497,27 +2292,6 @@
 It's important to remember that this is just one way to test the contract between equals() and hashCode() using JUnit theory and different scenarios might require different test cases.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>Did not check null points or points with similar values</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Lacks testing knowledge</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">The given code correctly finds the last zero element in the array by iterating through the array in reverse order. However, it does not handle the case where there are multiple zeroes in the array. In such a case, it will return the index of the first zero it encounters instead of the last one. To fix this, you can modify the code to store the index of the last zero encountered in a separate variable, and update that variable every time a zero is encountered. Then, return that variable after the loop.
 ```
    public static int lastZero (int[] x)
@@ -3022,9 +2796,6 @@
     <t>Confidence.2</t>
   </si>
   <si>
-    <t>Explanation correct from the prespective that assumption about equality is not correct to the tester</t>
-  </si>
-  <si>
     <t>A test case that results in an error, but not a failure is passing a null value to the function as an argument, for example:
 lastZero(null);
 This will throw a NullPointerException because the code checks for a null value and throws an exception if the input array is null. This is an error because it indicates that something unexpected happened in the program, but it's not a failure because the program will not crash or halt, it will just throw an exception and the program can continue executing other lines of code after catching the exception.
@@ -3036,14 +2807,193 @@
 Detects test from the commented code</t>
   </si>
   <si>
-    <t>Solution code is faulty.</t>
+    <t xml:space="preserve">The first error state for the test case where a null value is passed to the function as an argument, for example:
+lastZero(null);
+The error state is a NullPointerException being thrown. This error state occurs when the code attempts to access elements of the input array, but the array is null, so the program throws an exception.
+The complete state of the error would be:
+The program counter is pointing at the line where the exception is thrown
+The exception message is "null"
+The stack trace will show the method lastZero(int[] x) as the location where the exception occurred
+The program continues to execute other lines of code after catching the exception, if it is handled properly.
+It is worth noting that this error state is handled explicitly by the code, it will throw the exception if the input is null, so it is not a failure but it is an error.
+</t>
+  </si>
+  <si>
+    <t>Wrong test case</t>
+  </si>
+  <si>
+    <t>No test case</t>
+  </si>
+  <si>
+    <t>The given test case is:
+int[] x = {-3, -2, 0, 1, 4};
+int result = oddOrPos(x);
+assert result == 3;
+In this test case, the first error state would not occur because the input array x is non-null. The method implementation includes a null check to check if the input array is null or not, if it is null it will throw a NullPointerException. Since the input array is non-null, the method will execute as expected and the first error state will not occur.
+It is worth noting that the test case also includes an assertion that compares the returned result from the method with the expected value of 3, if the returned value is not 3 it will result in an assertion error and the program will stop execution.</t>
+  </si>
+  <si>
+    <t>Here is an implementation of the repaired code that includes a null check for the input array:
+public static int oddOrPos (int[] x) {
+      if (x == null) {
+         throw new NullPointerException("Input array cannot be null");
+      }
+      int count = 0;
+      for (int i = 0; i &lt; x.length; i++) {
+         if (x[i]%2 == 1 || x[i] &gt; 0) {
+            count++;
+         }
+      }
+      return count;
+   }
+And here is the test case that verifies that the given test now produces the expected output:
+Copy code
+int[] x = {-3, -2, 0, 1, 4};
+int result = oddOrPos(x);
+assert result == 3;
+As you can see, the method now includes a null check for the input array, which will ensure that the method will throw a NullPointerException if a null array is passed as an input. The test case that is provided will pass as the input array is non-null and the expected output is 3 which is being asserted against the returned result.
+In addition, if you are running this code on a Java development environment such as eclipse, it will give you a message that the test passed and you can see it on the console.</t>
+  </si>
+  <si>
+    <t>The given code uses the BigDecimal class, which has an inconsistency between its equals() and compareTo() methods. Specifically, x.equals(y) returns false, but x.compareTo(y) returns 0, indicating that they are equal. This inconsistency causes problems when using BigDecimal objects with certain types of collections, such as TreeSet and HashSet.
+In the given code, a TreeSet is created and both x and y are added to it. Since TreeSet uses the compareTo() method for ordering and comparison, the two BigDecimal objects are considered equal and only one element is added to the set. On the other hand, a HashSet is created and both x and y are added to it. Since HashSet uses the equals() method for comparison, the two BigDecimal objects are considered different and both are added to the set.
+To fix this fault, one approach would be to override the equals() method in the BigDecimal class to use the compareTo() method instead. Alternatively, a custom comparator that uses the compareTo() method could be provided when creating the TreeSet and HashSet collections.
+For example:
+public class BigDecimalTest {
+    BigDecimal x = new BigDecimal ("1.0");
+    BigDecimal y = new BigDecimal ("1.00");
+    //override equals method
+    @Override
+    public boolean equals(Object obj) {
+        if(obj instanceof BigDecimal) {
+            return this.compareTo((BigDecimal) obj) == 0;
+        }
+        return false;
+    }
+    // Fact: x.equals (y) should now return true, and x.compareTo (y) == 0
+    Set &lt;BigDecimal&gt; BigDecimalTree = new TreeSet &lt;BigDecimal&gt; ();
+    BigDecimalTree.add (x);
+    BigDecimalTree.add (y);
+    // TreeSet uses compareTo(), so BigDecimalTree will now have 1 element
+    Set &lt;BigDecimal&gt; BigDecimalHash = new HashSet &lt;BigDecimal&gt; ();
+    BigDecimalHash.add (x);
+    BigDecimalHash.add (y);
+    // HashSet uses equals(), so BigDecimalHash will now have 1 element
+    }
+    // Test: System.out.println ("BigDecimalTree = " + BigDecimalTree);
+    // System.out.println ("BigDecimalHash = " + BigDecimalHash);
+    // Expected: BigDecimalTree = 1; BigDecimalHash = 1
+    // See Java Doc for add() in Set Interface
+This modification will ensure that the equals() method will return true when comparing x and y and fix the inconsistency between equals() and compareTo() methods in the BigDecimal class.</t>
+  </si>
+  <si>
+    <t>It is not possible to give a test case that does not execute the fault because the fault is inherent in the way that the BigDecimal class is implemented. The equals() and compareTo() methods in the BigDecimal class return different results for certain values, which causes problems when using BigDecimal objects with certain types of collections, such as TreeSet and HashSet.
+However, once the equals method is overriden as described in (a) with the compareTo method, the test case will be successful.
+For example:
+BigDecimal x = new BigDecimal ("1.0");
+BigDecimal y = new BigDecimal ("1.00");
+Set &lt;BigDecimal&gt; BigDecimalTree = new TreeSet &lt;BigDecimal&gt; ();
+BigDecimalTree.add (x);
+BigDecimalTree.add (y);
+assertEquals(1,BigDecimalTree.size());
+Set &lt;BigDecimal&gt; BigDecimalHash = new HashSet &lt;BigDecimal&gt; ();
+BigDecimalHash.add (x);
+BigDecimalHash.add (y);
+assertEquals(1,BigDecimalHash.size());
+In this test case, the size of BigDecimalTree and BigDecimalHash should be 1, this means that only one element is added to each of them, which is expected.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the given example, the problem is that the BigDecimal class's equals() and compareTo() methods are inconsistent. The code creates two BigDecimal objects, x and y, with the values "1.0" and "1.00" respectively. Even though x and y are not equal according to the equals() method (!x.equals(y)), the compareTo() method returns 0, indicating that they are equal.
+When these objects are added to a TreeSet, the set uses the compareTo() method to determine equality, so only one element is added to the set. However, when added to a HashSet, the set uses the equals() method, so both x and y are added to the set.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>A test case that executes this fault but does not result in an error state would be to create two BigDecimal objects with slightly different values,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and add them to both a TreeSet and a HashSet. The output of the test would show that the TreeSet only has one element, while the HashSet has two elements, which would demonstrate the inconsistency between the equals() and compareTo() methods in the BigDecimal class.</t>
+    </r>
+  </si>
+  <si>
+    <t>APC or AIC?
+Did not talk about the exact line
+Treats error as exception/crash</t>
+  </si>
+  <si>
+    <t>As I mentioned before, one approach to repair the fault in the code is to override the equals() method in the BigDecimal class to use the compareTo() method instead.
+Here is the modified code:
+public class BigDecimalTest {
+    BigDecimal x = new BigDecimal ("1.0");
+    BigDecimal y = new BigDecimal ("1.00");
+    //override equals method
+    @Override
+    public boolean equals(Object obj) {
+        if(obj instanceof BigDecimal) {
+            return this.compareTo((BigDecimal) obj) == 0;
+        }
+        return false;
+    }
+    // Fact: x.equals (y) should now return true, and x.compareTo (y) == 0
+    Set &lt;BigDecimal&gt; BigDecimalTree = new TreeSet &lt;BigDecimal&gt; ();
+    BigDecimalTree.add (x);
+    BigDecimalTree.add (y);
+    // TreeSet uses compareTo(), so BigDecimalTree will now have 1 element
+    Set &lt;BigDecimal&gt; BigDecimalHash = new HashSet &lt;BigDecimal&gt; ();
+    BigDecimalHash.add (x);
+    BigDecimalHash.add (y);
+    // HashSet uses equals(), so BigDecimalHash will now have 1 element
+    }
+    // Test: System.out.println ("BigDecimalTree = " + BigDecimalTree);
+    // System.out.println ("BigDecimalHash = " + BigDecimalHash);
+    // Expected: BigDecimalTree = 1; BigDecimalHash = 1
+With this modification, the test case that was provided will now produce the expected output.
+BigDecimal x = new BigDecimal ("1.0");
+BigDecimal y = new BigDecimal ("1.00");
+Set &lt;BigDecimal&gt; BigDecimalTree = new TreeSet &lt;BigDecimal&gt; ();
+BigDecimalTree.add (x);
+BigDecimalTree.add (y);
+assertEquals(1,BigDecimalTree.size());
+Set &lt;BigDecimal&gt; BigDecimalHash = new HashSet &lt;BigDecimal&gt; ();
+BigDecimalHash.add (x);
+BigDecimalHash.add (y);
+assertEquals(1,BigDecimalHash.size());
+In this test case, the size of BigDecimalTree and BigDecimalHash should be 1, this means that only one element is added to each of them, which is expected.
+I apologize but as a language model AI I am not able to provide you with a screenshot or any other evidence, but you can run the code and see that it works as expected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is possible to give a test case that executes the fault but does not result in an error state.
+For example, the following test case:
+Point p = new Point (1,2);
+ColorPoint cp1 = new ColorPoint (1,2,RED);
+ColorPoint cp2 = new ColorPoint (1,2,BLUE);
+p.equals (cp1); // Test 1: Result = true;
+This test case will execute the fault because the equals method in the ColorPoint class does not properly check for equality of all relevant fields, including the color field, when comparing ColorPoint objects. However, it does not result in an error state because the result of the comparison is true.
+This is because the equals method of Point class is being used to compare the Point and ColorPoint object, it checks for equality of x and y fields and hence the comparison returns true.
+Even though this test case does not result in an error state, it is still problematic because it can lead to unexpected behavior and bugs in the program, as it is returning true when it should be false.
+</t>
+  </si>
+  <si>
+    <t>APC sounds more appropriate here. The chatgpt solution looks correct except for the Point vs. Object parameter type. The solution is correct that Object is likely better but JUnit theory test and DataPoints otherwise look okay in ChatGPT's answer. (ChatGPT's answer should have perhaps included null too though)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3083,8 +3033,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3100,12 +3061,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3167,7 +3122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3184,14 +3139,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3202,8 +3157,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3522,12 +3480,12 @@
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" style="1"/>
     <col min="3" max="3" width="45.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.1640625" style="1" customWidth="1"/>
@@ -3556,23 +3514,25 @@
     <col min="28" max="28" width="14.1640625" style="1" customWidth="1"/>
     <col min="29" max="29" width="12.33203125" style="1" customWidth="1"/>
     <col min="30" max="30" width="12.83203125" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="8.83203125" style="1"/>
+    <col min="31" max="31" width="8.83203125" style="1"/>
+    <col min="32" max="32" width="20" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -3585,9 +3545,9 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="J1" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -3599,7 +3559,7 @@
       <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>12</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -3611,7 +3571,7 @@
       <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="10" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="2" t="s">
@@ -3624,9 +3584,9 @@
         <v>19</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="W1" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="W1" s="10" t="s">
         <v>20</v>
       </c>
       <c r="X1" s="2" t="s">
@@ -3638,7 +3598,7 @@
       <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AA1" s="10" t="s">
         <v>24</v>
       </c>
       <c r="AB1" s="2" t="s">
@@ -3651,9 +3611,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>211</v>
+    <row r="2" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>28</v>
@@ -3665,19 +3625,19 @@
         <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>248</v>
+        <v>264</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>42</v>
@@ -3689,7 +3649,7 @@
         <v>44</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>43</v>
@@ -3701,13 +3661,10 @@
         <v>45</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>291</v>
+        <v>41</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>47</v>
@@ -3728,9 +3685,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>211</v>
+    <row r="3" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
@@ -3742,7 +3699,7 @@
         <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>40</v>
@@ -3753,8 +3710,8 @@
       <c r="H3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>248</v>
+      <c r="I3" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>51</v>
@@ -3766,7 +3723,7 @@
         <v>41</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>40</v>
@@ -3802,9 +3759,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>211</v>
+    <row r="4" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>31</v>
@@ -3816,7 +3773,7 @@
         <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>40</v>
@@ -3824,8 +3781,8 @@
       <c r="G4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>248</v>
+      <c r="I4" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>55</v>
@@ -3837,7 +3794,7 @@
         <v>41</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>40</v>
@@ -3873,9 +3830,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>211</v>
+    <row r="5" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>33</v>
@@ -3887,72 +3844,69 @@
         <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>44</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>248</v>
+        <v>205</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>59</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="S5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="X5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="AB5" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AC5" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>211</v>
+    <row r="6" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
@@ -3964,7 +3918,7 @@
         <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>222</v>
+        <v>265</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>40</v>
@@ -3973,50 +3927,50 @@
         <v>41</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>248</v>
+        <v>205</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="S6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="W6" s="1" t="s">
+      <c r="X6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="X6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA6" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="AB6" s="1" t="s">
         <v>40</v>
       </c>
@@ -4024,9 +3978,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>211</v>
+    <row r="7" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>37</v>
@@ -4038,250 +3992,247 @@
         <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>248</v>
+        <v>41</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="O7" s="1" t="s">
+      <c r="N7" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="O7" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="S7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="W7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U7" s="1" t="s">
+      <c r="X7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="W7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA7" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AB7" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>212</v>
+    <row r="8" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>248</v>
-      </c>
       <c r="J8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AB8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC8" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="388" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>212</v>
+    <row r="9" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>248</v>
+        <v>205</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC9" s="1" t="s">
+      <c r="AB9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC9" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="388" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>212</v>
+    <row r="10" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>248</v>
+        <v>205</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>40</v>
@@ -4290,7 +4241,7 @@
         <v>41</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>40</v>
@@ -4299,7 +4250,7 @@
         <v>41</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>40</v>
@@ -4308,7 +4259,7 @@
         <v>41</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X10" s="3" t="s">
         <v>40</v>
@@ -4317,7 +4268,7 @@
         <v>41</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="AB10" s="3" t="s">
         <v>40</v>
@@ -4326,21 +4277,21 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="388" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>212</v>
+    <row r="11" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>40</v>
@@ -4349,13 +4300,13 @@
         <v>44</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>248</v>
+        <v>205</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>40</v>
@@ -4364,7 +4315,7 @@
         <v>44</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>40</v>
@@ -4373,152 +4324,137 @@
         <v>44</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T11" s="3" t="s">
         <v>41</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="3" t="s">
         <v>41</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC11" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="388" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>212</v>
+    <row r="12" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>248</v>
+        <v>211</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>93</v>
+        <v>240</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>212</v>
+    <row r="13" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>248</v>
+        <v>211</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>40</v>
@@ -4526,11 +4462,9 @@
       <c r="L13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="M13" s="3"/>
       <c r="N13" s="1" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>40</v>
@@ -4538,23 +4472,18 @@
       <c r="P13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Q13" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="Q13" s="3"/>
       <c r="R13" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>43</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="X13" s="3" t="s">
         <v>40</v>
@@ -4562,37 +4491,32 @@
       <c r="Y13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="Z13" s="3"/>
       <c r="AA13" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="AB13" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>213</v>
+    <row r="14" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>231</v>
+        <v>270</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>43</v>
@@ -4601,13 +4525,13 @@
         <v>44</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>215</v>
+        <v>202</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>43</v>
@@ -4616,7 +4540,7 @@
         <v>44</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>43</v>
@@ -4625,7 +4549,7 @@
         <v>44</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>43</v>
@@ -4634,7 +4558,7 @@
         <v>44</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="X14" s="1" t="s">
         <v>43</v>
@@ -4643,7 +4567,7 @@
         <v>44</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="AB14" s="1" t="s">
         <v>43</v>
@@ -4652,110 +4576,110 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>213</v>
+    <row r="15" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>44</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>216</v>
+        <v>202</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>44</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P15" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P15" s="3" t="s">
         <v>44</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>41</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AB15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC15" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>213</v>
+    <row r="16" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>40</v>
@@ -4764,57 +4688,57 @@
         <v>41</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P16" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="T16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>120</v>
+        <v>272</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>213</v>
+    <row r="17" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>43</v>
@@ -4823,13 +4747,13 @@
         <v>44</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>40</v>
@@ -4838,19 +4762,16 @@
         <v>41</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="O17" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="O17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>123</v>
+      <c r="P17" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>40</v>
@@ -4859,7 +4780,7 @@
         <v>41</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="X17" s="1" t="s">
         <v>40</v>
@@ -4867,52 +4788,46 @@
       <c r="Y17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Z17" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="AA17" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD17" s="1" t="s">
-        <v>288</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>213</v>
+    <row r="18" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>69</v>
+        <v>214</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>215</v>
+        <v>273</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>40</v>
@@ -4920,11 +4835,8 @@
       <c r="L18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="N18" s="1" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>40</v>
@@ -4932,11 +4844,8 @@
       <c r="P18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Q18" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="R18" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="S18" s="3" t="s">
         <v>40</v>
@@ -4944,11 +4853,8 @@
       <c r="T18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="U18" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="W18" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="X18" s="3" t="s">
         <v>40</v>
@@ -4956,11 +4862,8 @@
       <c r="Y18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Z18" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="AA18" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="AB18" s="3" t="s">
         <v>40</v>
@@ -4968,114 +4871,96 @@
       <c r="AC18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AD18" s="1" t="s">
-        <v>128</v>
-      </c>
     </row>
-    <row r="19" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>213</v>
+    <row r="19" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>237</v>
+        <v>274</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="X19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z19" s="1" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="AB19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD19" s="1" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>214</v>
+    <row r="20" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>198</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>46</v>
@@ -5084,87 +4969,72 @@
         <v>41</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z20" s="1" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>214</v>
+    <row r="21" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>198</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>43</v>
@@ -5173,31 +5043,31 @@
         <v>44</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>216</v>
+        <v>202</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>44</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P21" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>44</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>40</v>
@@ -5206,19 +5076,16 @@
         <v>41</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="Y21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Z21" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="AA21" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="AB21" s="1" t="s">
         <v>43</v>
@@ -5227,63 +5094,63 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>214</v>
+    <row r="22" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>198</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L22" s="1" t="s">
+      <c r="K22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>41</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P22" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P22" s="3" t="s">
         <v>41</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T22" s="3" t="s">
         <v>41</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="X22" s="3" t="s">
         <v>40</v>
@@ -5292,7 +5159,7 @@
         <v>41</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="AB22" s="3" t="s">
         <v>40</v>
@@ -5301,72 +5168,72 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>214</v>
+    <row r="23" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>198</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>216</v>
+        <v>205</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L23" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P23" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="T23" s="1" t="s">
         <v>41</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="X23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y23" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="AB23" s="1" t="s">
         <v>40</v>
@@ -5375,21 +5242,21 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>214</v>
+    <row r="24" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>198</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>43</v>
@@ -5398,13 +5265,13 @@
         <v>44</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>216</v>
+        <v>146</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>43</v>
@@ -5413,7 +5280,7 @@
         <v>44</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>43</v>
@@ -5422,7 +5289,7 @@
         <v>44</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="S24" s="1" t="s">
         <v>43</v>
@@ -5431,7 +5298,7 @@
         <v>44</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="X24" s="1" t="s">
         <v>43</v>
@@ -5440,7 +5307,7 @@
         <v>44</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="AB24" s="1" t="s">
         <v>43</v>
@@ -5448,25 +5315,22 @@
       <c r="AC24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AD24" s="1" t="s">
-        <v>164</v>
-      </c>
     </row>
-    <row r="25" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>214</v>
+    <row r="25" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>198</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>40</v>
@@ -5475,13 +5339,13 @@
         <v>41</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>216</v>
+        <v>223</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>40</v>
@@ -5490,7 +5354,7 @@
         <v>41</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>40</v>
@@ -5499,7 +5363,7 @@
         <v>41</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="S25" s="1" t="s">
         <v>40</v>
@@ -5508,122 +5372,116 @@
         <v>41</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z25" s="1" t="s">
-        <v>168</v>
+        <v>41</v>
       </c>
       <c r="AA25" s="1" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AC25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD25" s="1" t="s">
-        <v>168</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
+    <row r="26" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
         <v>3.9</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>216</v>
+        <v>225</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L26" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M26"/>
       <c r="N26" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P26" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="Q26"/>
       <c r="R26" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="S26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T26" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="U26"/>
       <c r="V26"/>
       <c r="W26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="X26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y26" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="Z26"/>
       <c r="AA26" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="AB26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC26" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="AD26"/>
     </row>
-    <row r="27" spans="1:30" ht="340" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
+    <row r="27" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
         <v>3.9</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>43</v>
@@ -5631,11 +5489,11 @@
       <c r="G27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>248</v>
+      <c r="I27" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>43</v>
@@ -5645,7 +5503,7 @@
       </c>
       <c r="M27"/>
       <c r="N27" s="1" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>43</v>
@@ -5655,7 +5513,7 @@
       </c>
       <c r="Q27"/>
       <c r="R27" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>43</v>
@@ -5666,7 +5524,7 @@
       <c r="U27"/>
       <c r="V27"/>
       <c r="W27" s="1" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="X27" s="1" t="s">
         <v>43</v>
@@ -5676,7 +5534,7 @@
       </c>
       <c r="Z27"/>
       <c r="AA27" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="AB27" s="1" t="s">
         <v>43</v>
@@ -5686,264 +5544,252 @@
       </c>
       <c r="AD27"/>
     </row>
-    <row r="28" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
+    <row r="28" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
         <v>3.9</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>248</v>
+        <v>227</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L28" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L28" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M28"/>
       <c r="N28" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P28" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P28" s="1" t="s">
         <v>44</v>
       </c>
       <c r="Q28"/>
       <c r="R28" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="S28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T28" s="1" t="s">
         <v>44</v>
       </c>
       <c r="U28"/>
       <c r="V28"/>
       <c r="W28" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="X28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y28" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="X28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y28" s="1" t="s">
         <v>44</v>
       </c>
       <c r="Z28"/>
       <c r="AA28" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AB28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC28" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC28" s="1" t="s">
         <v>44</v>
       </c>
       <c r="AD28"/>
     </row>
-    <row r="29" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
+    <row r="29" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
         <v>3.9</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>248</v>
+        <v>228</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L29" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M29"/>
       <c r="N29" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P29" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="Q29"/>
       <c r="R29" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="S29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T29" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="U29"/>
       <c r="V29"/>
       <c r="W29" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="X29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y29" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="X29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="Z29"/>
       <c r="AA29" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AB29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC29" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC29" s="1" t="s">
         <v>44</v>
       </c>
       <c r="AD29"/>
     </row>
-    <row r="30" spans="1:30" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A30" s="7">
+    <row r="30" spans="1:30" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
         <v>3.9</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>248</v>
+        <v>68</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>46</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>192</v>
+        <v>68</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="O30" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="O30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P30" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="P30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q30" s="3"/>
       <c r="R30" s="1" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="S30" s="1" t="s">
         <v>46</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="U30" s="1" t="s">
-        <v>192</v>
+        <v>68</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="X30" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="X30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y30" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z30" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="Y30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z30" s="3"/>
       <c r="AA30" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AB30" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC30" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD30" s="3" t="s">
-        <v>192</v>
-      </c>
+      <c r="AC30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD30" s="3"/>
     </row>
-    <row r="31" spans="1:30" ht="136" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
+    <row r="31" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
         <v>5.0999999999999996</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>46</v>
@@ -5952,13 +5798,13 @@
         <v>41</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>215</v>
+        <v>194</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>46</v>
@@ -5966,11 +5812,8 @@
       <c r="L31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M31" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="N31" s="1" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>46</v>
@@ -5978,11 +5821,8 @@
       <c r="P31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q31" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="R31" s="1" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="S31" s="1" t="s">
         <v>46</v>
@@ -5990,11 +5830,8 @@
       <c r="T31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U31" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="W31" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="X31" s="1" t="s">
         <v>46</v>
@@ -6002,11 +5839,8 @@
       <c r="Y31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Z31" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="AA31" s="1" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="AB31" s="1" t="s">
         <v>46</v>
@@ -6014,25 +5848,22 @@
       <c r="AC31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AD31" s="1" t="s">
-        <v>210</v>
-      </c>
     </row>
-    <row r="32" spans="1:30" ht="170" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
+    <row r="32" spans="1:30" ht="388" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
         <v>5.0999999999999996</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>43</v>
@@ -6040,11 +5871,11 @@
       <c r="G32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I32" s="6" t="s">
-        <v>215</v>
+      <c r="I32" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>43</v>
@@ -6053,7 +5884,7 @@
         <v>44</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="O32" s="1" t="s">
         <v>43</v>
@@ -6062,7 +5893,7 @@
         <v>44</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="S32" s="1" t="s">
         <v>43</v>
@@ -6071,7 +5902,7 @@
         <v>44</v>
       </c>
       <c r="W32" s="1" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="X32" s="1" t="s">
         <v>43</v>
@@ -6080,7 +5911,7 @@
         <v>44</v>
       </c>
       <c r="AA32" s="1" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="AB32" s="1" t="s">
         <v>43</v>

</xml_diff>